<commit_message>
OOH DB Connection changed
</commit_message>
<xml_diff>
--- a/Orchestrator2022/OOH S9/OOH_S9_Dispatcher.2023.10.13/lib/net45/Data/Config.xlsx
+++ b/Orchestrator2022/OOH S9/OOH_S9_Dispatcher.2023.10.13/lib/net45/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.OOHPBTDIGS9\Documents\NA-Automation\OOH S9\ORC Folder RE\OOH_S9_Dispatcher.2023.10.13\lib\net45\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NTMGRM.OOHPBTDIGS9\Documents\NA-Automation\OOH S9\OOH_S9_Dispatcher.2023.10.13\lib\net45\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD43FEF-9FE4-492A-A416-668BA52C496F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8DDC59-DD6E-4ABC-9C69-126F59BCC34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>DB_ConnectionProd</t>
   </si>
   <si>
-    <t>Data Source=eussqsvgrmusafinance01.database.windows.net;Initial Catalog=eussqdbgrmusaapooh01;User ID=NA_AP_OOH_DBAUSR_01;Password=n28UxD8NVZAqdFMjBHnd</t>
-  </si>
-  <si>
     <t>OOHS9</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t>GMUSA_OOHS9</t>
+  </si>
+  <si>
+    <t>Data Source=eussqlsrvgrmusafinanceprd01.database.windows.net;Initial Catalog=eussqldbgrmusafinanceoohprd01;User ID=NA_AP_OOH_DBAUSR_PRD_01;Password=68RaM#wp7Dcch7Khyg</t>
   </si>
 </sst>
 </file>
@@ -547,7 +547,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -644,7 +644,7 @@
         <v>35</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -652,18 +652,18 @@
         <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4051,15 +4051,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="7f25b792-b2ba-4b5c-8669-b39a27555406" xsi:nil="true"/>
@@ -4069,6 +4060,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4091,14 +4091,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6ABAFDB-5512-4091-8996-86783A07DFD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1872259B-7FE8-4429-8338-A7D085551264}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4107,4 +4099,12 @@
     <ds:schemaRef ds:uri="649a79cd-06e4-47a3-aac9-21cb806f3675"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6ABAFDB-5512-4091-8996-86783A07DFD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>